<commit_message>
Added interactive/script column into the spreadsheet
</commit_message>
<xml_diff>
--- a/DataVis_app_list.xlsx
+++ b/DataVis_app_list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koleinik\Dropbox (BOSTON UNIVERSITY)\Projects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koleinik\Dropbox (BOSTON UNIVERSITY)\Digital Humanities\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="114">
   <si>
     <t>Data Visualization Tools Spreadsheet</t>
   </si>
@@ -350,13 +350,31 @@
   </si>
   <si>
     <t>Professional quality vector graphics . It is used  for creating a wide variety of graphics such as illustrations, icons, logos, diagrams, maps and web graphics. Inkscape uses the W3C open standard SVG (Scalable Vector Graphics) as its native format, and is free and open-source software.</t>
+  </si>
+  <si>
+    <t>Useful links:</t>
+  </si>
+  <si>
+    <t>https://source.opennews.org/articles/what-i-learned-recreating-one-chart-using-24-tools/</t>
+  </si>
+  <si>
+    <t>What I Learned Recreating One Chart Using 24 Tools</t>
+  </si>
+  <si>
+    <t>Interactive/Scripting</t>
+  </si>
+  <si>
+    <t>interactive</t>
+  </si>
+  <si>
+    <t>script</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -399,6 +417,22 @@
       <b/>
       <i/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -512,7 +546,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -557,6 +591,8 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -838,31 +874,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C34" sqref="C34"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.1796875" customWidth="1"/>
     <col min="2" max="2" width="29.6328125" customWidth="1"/>
-    <col min="3" max="3" width="14.7265625" customWidth="1"/>
-    <col min="4" max="4" width="49" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.6328125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="44.6328125" customWidth="1"/>
-    <col min="7" max="7" width="26.6328125" customWidth="1"/>
+    <col min="3" max="4" width="19.26953125" customWidth="1"/>
+    <col min="5" max="5" width="49" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.6328125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="44.6328125" customWidth="1"/>
+    <col min="8" max="8" width="26.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="26" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:7" ht="26" x14ac:dyDescent="0.6">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:6" s="3" customFormat="1" ht="33.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:7" s="3" customFormat="1" ht="33.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="19" t="s">
         <v>1</v>
       </c>
@@ -872,17 +908,20 @@
       <c r="C3" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="E3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="F3" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="G3" s="19" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="80.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="80.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="21" t="s">
         <v>5</v>
       </c>
@@ -890,17 +929,20 @@
         <v>7</v>
       </c>
       <c r="C4" s="16"/>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E4" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="F4" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="G4" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
         <v>8</v>
       </c>
@@ -910,17 +952,18 @@
       <c r="C5" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4"/>
+      <c r="E5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="22" t="s">
         <v>12</v>
       </c>
@@ -930,17 +973,18 @@
       <c r="C6" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4"/>
+      <c r="E6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="22" t="s">
         <v>16</v>
       </c>
@@ -950,17 +994,18 @@
       <c r="C7" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4"/>
+      <c r="E7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="22" t="s">
         <v>45</v>
       </c>
@@ -970,17 +1015,18 @@
       <c r="C8" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4"/>
+      <c r="E8" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="22" t="s">
         <v>25</v>
       </c>
@@ -990,17 +1036,18 @@
       <c r="C9" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4"/>
+      <c r="E9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="22" t="s">
         <v>77</v>
       </c>
@@ -1008,17 +1055,20 @@
         <v>80</v>
       </c>
       <c r="C10" s="4"/>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="90" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="23" t="s">
         <v>31</v>
       </c>
@@ -1028,17 +1078,18 @@
       <c r="C11" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="8"/>
+      <c r="E11" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="90" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="23" t="s">
         <v>74</v>
       </c>
@@ -1048,17 +1099,18 @@
       <c r="C12" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="8"/>
+      <c r="E12" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="E12" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="8" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="53" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="53" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="24" t="s">
         <v>28</v>
       </c>
@@ -1066,15 +1118,16 @@
         <v>29</v>
       </c>
       <c r="C13" s="10"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11" t="s">
+      <c r="D13" s="10"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="G13" s="12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="24" t="s">
         <v>39</v>
       </c>
@@ -1082,17 +1135,18 @@
         <v>37</v>
       </c>
       <c r="C14" s="10"/>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="10"/>
+      <c r="E14" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="24" t="s">
         <v>40</v>
       </c>
@@ -1102,17 +1156,18 @@
       <c r="C15" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="10"/>
+      <c r="E15" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="F15" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="G15" s="12" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A16" s="24" t="s">
         <v>61</v>
       </c>
@@ -1120,17 +1175,18 @@
         <v>64</v>
       </c>
       <c r="C16" s="10"/>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="10"/>
+      <c r="E16" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E16" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" s="10" t="s">
+      <c r="F16" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" s="10" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A17" s="24" t="s">
         <v>66</v>
       </c>
@@ -1138,17 +1194,18 @@
         <v>68</v>
       </c>
       <c r="C17" s="10"/>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="10"/>
+      <c r="E17" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="E17" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A18" s="24" t="s">
         <v>101</v>
       </c>
@@ -1156,17 +1213,18 @@
         <v>102</v>
       </c>
       <c r="C18" s="10"/>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="10"/>
+      <c r="E18" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="E18" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" s="10" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A19" s="24" t="s">
         <v>60</v>
       </c>
@@ -1174,17 +1232,18 @@
         <v>59</v>
       </c>
       <c r="C19" s="10"/>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="10"/>
+      <c r="E19" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="E19" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="10" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A20" s="25" t="s">
         <v>21</v>
       </c>
@@ -1194,17 +1253,20 @@
       <c r="C20" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="E20" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="E20" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="F20" s="15" t="s">
+      <c r="F20" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" s="15" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="25" t="s">
         <v>49</v>
       </c>
@@ -1214,17 +1276,20 @@
       <c r="C21" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="E21" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="E21" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="F21" s="15" t="s">
+      <c r="F21" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" s="15" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="25" t="s">
         <v>53</v>
       </c>
@@ -1234,17 +1299,20 @@
       <c r="C22" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="D22" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="E22" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="E22" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="F22" s="13" t="s">
+      <c r="F22" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" s="13" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A23" s="25" t="s">
         <v>69</v>
       </c>
@@ -1254,17 +1322,20 @@
       <c r="C23" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="D23" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="E23" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="E23" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="F23" s="13" t="s">
+      <c r="F23" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23" s="13" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="25" t="s">
         <v>85</v>
       </c>
@@ -1274,17 +1345,18 @@
       <c r="C24" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="D24" s="13"/>
+      <c r="E24" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="E24" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="F24" s="13" t="s">
+      <c r="F24" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" s="13" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="25" t="s">
         <v>89</v>
       </c>
@@ -1294,17 +1366,20 @@
       <c r="C25" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="D25" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="E25" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="E25" s="14" t="s">
+      <c r="F25" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="F25" s="15" t="s">
+      <c r="G25" s="15" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="83" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="83" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="27" t="s">
         <v>105</v>
       </c>
@@ -1314,79 +1389,95 @@
       <c r="C26" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="D26" s="13"/>
+      <c r="E26" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="E26" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="F26" s="13" t="s">
+      <c r="F26" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G26" s="13" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="83" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="83" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="25"/>
       <c r="B27" s="13"/>
       <c r="C27" s="13"/>
-      <c r="D27" s="14"/>
+      <c r="D27" s="13"/>
       <c r="E27" s="14"/>
-      <c r="F27" s="13"/>
-    </row>
-    <row r="28" spans="1:6" ht="83" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F27" s="14"/>
+      <c r="G27" s="13"/>
+    </row>
+    <row r="28" spans="1:7" ht="83" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="25"/>
       <c r="B28" s="13"/>
       <c r="C28" s="13"/>
-      <c r="D28" s="14"/>
+      <c r="D28" s="13"/>
       <c r="E28" s="14"/>
-      <c r="F28" s="13"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F28" s="14"/>
+      <c r="G28" s="13"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="26" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="26" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="26" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="26" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="26" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="26" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="26" t="s">
         <v>100</v>
       </c>
     </row>
+    <row r="41" spans="1:5" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A41" s="29" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B42" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="E42" t="s">
+        <v>109</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F4" r:id="rId1"/>
-    <hyperlink ref="F5" r:id="rId2"/>
-    <hyperlink ref="F6" r:id="rId3" display="http://dygraphs.com/ "/>
-    <hyperlink ref="F7" r:id="rId4"/>
-    <hyperlink ref="F20" r:id="rId5"/>
-    <hyperlink ref="F13" r:id="rId6"/>
-    <hyperlink ref="F15" r:id="rId7"/>
-    <hyperlink ref="F8" r:id="rId8"/>
-    <hyperlink ref="F21" r:id="rId9"/>
-    <hyperlink ref="F25" r:id="rId10"/>
+    <hyperlink ref="G4" r:id="rId1"/>
+    <hyperlink ref="G5" r:id="rId2"/>
+    <hyperlink ref="G6" r:id="rId3" display="http://dygraphs.com/ "/>
+    <hyperlink ref="G7" r:id="rId4"/>
+    <hyperlink ref="G20" r:id="rId5"/>
+    <hyperlink ref="G13" r:id="rId6"/>
+    <hyperlink ref="G15" r:id="rId7"/>
+    <hyperlink ref="G8" r:id="rId8"/>
+    <hyperlink ref="G21" r:id="rId9"/>
+    <hyperlink ref="G25" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId11"/>

</xml_diff>